<commit_message>
feat(insight): add product list endpoin
</commit_message>
<xml_diff>
--- a/backend/tests/data/吸尘器-sample.xlsx
+++ b/backend/tests/data/吸尘器-sample.xlsx
@@ -7364,8 +7364,8 @@
   <sheetPr/>
   <dimension ref="A1:CL103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="AV1" workbookViewId="0">
+      <selection activeCell="BC3" sqref="BC3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>

</xml_diff>